<commit_message>
[FIX] import and export user
</commit_message>
<xml_diff>
--- a/src/main/resources/template/Mau-danh-sach-nguoi-dung.xlsx
+++ b/src/main/resources/template/Mau-danh-sach-nguoi-dung.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xuant\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FALL 2023\Capstone\source_code\vms-server\src\main\resources\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD6DF676-C896-4BA0-8252-94B915B0FF87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59B37BA7-2720-4597-8D2A-C7F4672D45E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Email</t>
   </si>
   <si>
-    <t>STT</t>
-  </si>
-  <si>
     <t>Username</t>
   </si>
   <si>
@@ -55,13 +52,40 @@
   </si>
   <si>
     <t>DateOfBirth</t>
+  </si>
+  <si>
+    <t>MALE</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>sample</t>
+  </si>
+  <si>
+    <t>this</t>
+  </si>
+  <si>
+    <t>0912345678</t>
+  </si>
+  <si>
+    <t>sample@gmaail.com</t>
+  </si>
+  <si>
+    <t>2001-01-15</t>
+  </si>
+  <si>
+    <t>code1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,6 +115,14 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <scheme val="major"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -131,10 +163,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -145,8 +178,12 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -425,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -447,43 +484,81 @@
   <sheetData>
     <row r="1" spans="1:10" s="2" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
+      <c r="H2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="J1:J1048576" xr:uid="{58F2B368-7CC1-49A1-860E-2FAA38734BB5}">
       <formula1>"1,0"</formula1>
     </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576" xr:uid="{DD53565C-3360-49B9-A946-DEE6DC621845}">
+      <formula1>"MALE,FEMALE,OTHER"</formula1>
+    </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{7D287895-D3EB-4A82-9978-A9B2B9E4E236}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>